<commit_message>
FIX changed std_logic_vector to signed type for x, y and h
Issue arose because multiplication implemented
by VHDL libraries with std_logic_vector
is not signed multiplication
</commit_message>
<xml_diff>
--- a/vhdl/filter/fir/simulation.xlsx
+++ b/vhdl/filter/fir/simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Digital-Hardware-Modelling\vhdl\filter\fir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4770213C-D2AF-4A64-AE15-C8B7CBA750F6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D8940C8F-FC7E-472A-911C-320C02E71E25}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2352" windowWidth="23040" windowHeight="8484" xr2:uid="{79F3912B-60D2-46A9-A84E-4C5DD2F36FC7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="26">
   <si>
     <t>rst</t>
   </si>
@@ -620,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12858E77-0C5E-4420-971C-585D886428DF}">
-  <dimension ref="A1:AG1048576"/>
+  <dimension ref="A1:AG1048572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG23" sqref="AG23"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1550,7 +1550,9 @@
         <v>1</v>
       </c>
       <c r="AE11" s="21"/>
-      <c r="AF11" s="20"/>
+      <c r="AF11" s="20">
+        <v>1</v>
+      </c>
       <c r="AG11" s="22">
         <v>1</v>
       </c>
@@ -1630,7 +1632,9 @@
         <v>2</v>
       </c>
       <c r="AE12" s="21"/>
-      <c r="AF12" s="20"/>
+      <c r="AF12" s="20">
+        <v>1</v>
+      </c>
       <c r="AG12" s="22">
         <v>2</v>
       </c>
@@ -1710,7 +1714,9 @@
         <v>3</v>
       </c>
       <c r="AE13" s="21"/>
-      <c r="AF13" s="20"/>
+      <c r="AF13" s="20">
+        <v>1</v>
+      </c>
       <c r="AG13" s="22">
         <v>3</v>
       </c>
@@ -1790,7 +1796,9 @@
         <v>4</v>
       </c>
       <c r="AE14" s="21"/>
-      <c r="AF14" s="20"/>
+      <c r="AF14" s="20">
+        <v>1</v>
+      </c>
       <c r="AG14" s="22">
         <v>4</v>
       </c>
@@ -1870,7 +1878,9 @@
         <v>4</v>
       </c>
       <c r="AE15" s="21"/>
-      <c r="AF15" s="20"/>
+      <c r="AF15" s="20">
+        <v>1</v>
+      </c>
       <c r="AG15" s="22">
         <v>4</v>
       </c>
@@ -1950,7 +1960,9 @@
         <v>4</v>
       </c>
       <c r="AE16" s="21"/>
-      <c r="AF16" s="20"/>
+      <c r="AF16" s="20">
+        <v>1</v>
+      </c>
       <c r="AG16" s="22">
         <v>4</v>
       </c>
@@ -2030,7 +2042,9 @@
         <v>4</v>
       </c>
       <c r="AE17" s="21"/>
-      <c r="AF17" s="20"/>
+      <c r="AF17" s="20">
+        <v>1</v>
+      </c>
       <c r="AG17" s="22">
         <v>4</v>
       </c>
@@ -2085,16 +2099,16 @@
       </c>
       <c r="U18" s="13"/>
       <c r="V18" s="18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W18" s="18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X18" s="18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y18" s="19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z18" s="20"/>
       <c r="AA18" s="21">
@@ -2110,7 +2124,9 @@
         <v>4</v>
       </c>
       <c r="AE18" s="21"/>
-      <c r="AF18" s="20"/>
+      <c r="AF18" s="20">
+        <v>1</v>
+      </c>
       <c r="AG18" s="22">
         <v>4</v>
       </c>
@@ -2165,34 +2181,36 @@
       </c>
       <c r="U19" s="13"/>
       <c r="V19" s="18">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="W19" s="18">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="X19" s="18">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="Y19" s="19">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="Z19" s="20"/>
       <c r="AA19" s="21">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="AB19" s="21">
-        <v>65536</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="21">
-        <v>65537</v>
+        <v>1</v>
       </c>
       <c r="AD19" s="21">
-        <v>65538</v>
+        <v>2</v>
       </c>
       <c r="AE19" s="21"/>
-      <c r="AF19" s="20"/>
+      <c r="AF19" s="20">
+        <v>1</v>
+      </c>
       <c r="AG19" s="22">
-        <v>65538</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
@@ -2202,18 +2220,40 @@
       <c r="B20" s="13">
         <v>0</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="D20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0</v>
+      </c>
+      <c r="G20" s="13">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13">
+        <v>1</v>
+      </c>
       <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
+      <c r="J20" s="13">
+        <v>0</v>
+      </c>
+      <c r="K20" s="13">
+        <v>1</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" s="15">
+        <v>1</v>
+      </c>
+      <c r="O20" s="15">
+        <v>1</v>
+      </c>
+      <c r="P20" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="15">
+        <v>1</v>
+      </c>
       <c r="R20" s="16"/>
       <c r="S20" s="17">
         <v>-1</v>
@@ -2223,34 +2263,36 @@
       </c>
       <c r="U20" s="13"/>
       <c r="V20" s="18">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="W20" s="18">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="X20" s="18">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="Y20" s="19">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="Z20" s="20"/>
       <c r="AA20" s="21">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="AB20" s="21">
-        <v>131070</v>
+        <v>-2</v>
       </c>
       <c r="AC20" s="21">
-        <v>131071</v>
+        <v>-1</v>
       </c>
       <c r="AD20" s="21">
-        <v>131072</v>
+        <v>0</v>
       </c>
       <c r="AE20" s="21"/>
-      <c r="AF20" s="20"/>
+      <c r="AF20" s="20">
+        <v>1</v>
+      </c>
       <c r="AG20" s="22">
-        <v>131072</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
@@ -2260,18 +2302,40 @@
       <c r="B21" s="13">
         <v>0</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="D21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13">
+        <v>1</v>
+      </c>
       <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
+        <v>1</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" s="15">
+        <v>1</v>
+      </c>
+      <c r="O21" s="15">
+        <v>1</v>
+      </c>
+      <c r="P21" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="15">
+        <v>1</v>
+      </c>
       <c r="R21" s="16"/>
       <c r="S21" s="17">
         <v>-1</v>
@@ -2281,34 +2345,36 @@
       </c>
       <c r="U21" s="13"/>
       <c r="V21" s="18">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="W21" s="18">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="X21" s="18">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="Y21" s="19">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="Z21" s="20"/>
       <c r="AA21" s="21">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="AB21" s="21">
-        <v>131070</v>
+        <v>-2</v>
       </c>
       <c r="AC21" s="21">
-        <v>196605</v>
+        <v>-3</v>
       </c>
       <c r="AD21" s="21">
-        <v>196606</v>
+        <v>-2</v>
       </c>
       <c r="AE21" s="21"/>
-      <c r="AF21" s="20"/>
+      <c r="AF21" s="20">
+        <v>1</v>
+      </c>
       <c r="AG21" s="22">
-        <v>196606</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
@@ -2318,43 +2384,79 @@
       <c r="B22" s="13">
         <v>0</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="D22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0</v>
+      </c>
+      <c r="G22" s="13">
+        <v>1</v>
+      </c>
+      <c r="H22" s="13">
+        <v>1</v>
+      </c>
       <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
+      <c r="J22" s="13">
+        <v>0</v>
+      </c>
+      <c r="K22" s="13">
+        <v>1</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" s="15">
+        <v>1</v>
+      </c>
+      <c r="O22" s="15">
+        <v>1</v>
+      </c>
+      <c r="P22" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="15">
+        <v>1</v>
+      </c>
       <c r="R22" s="16"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
+      <c r="S22" s="17">
+        <v>-1</v>
+      </c>
+      <c r="T22" s="17">
+        <v>-1</v>
+      </c>
       <c r="U22" s="13"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="19"/>
+      <c r="V22" s="18">
+        <v>-1</v>
+      </c>
+      <c r="W22" s="18">
+        <v>-1</v>
+      </c>
+      <c r="X22" s="18">
+        <v>-1</v>
+      </c>
+      <c r="Y22" s="19">
+        <v>-1</v>
+      </c>
       <c r="Z22" s="20"/>
       <c r="AA22" s="21">
-        <v>65535</v>
+        <v>-1</v>
       </c>
       <c r="AB22" s="21">
-        <v>131070</v>
+        <v>-2</v>
       </c>
       <c r="AC22" s="21">
-        <v>196605</v>
+        <v>-3</v>
       </c>
       <c r="AD22" s="21">
-        <v>262140</v>
+        <v>-4</v>
       </c>
       <c r="AE22" s="21"/>
-      <c r="AF22" s="20"/>
+      <c r="AF22" s="20">
+        <v>1</v>
+      </c>
       <c r="AG22" s="22">
-        <v>262140</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
@@ -2364,160 +2466,83 @@
       <c r="B23" s="13">
         <v>0</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="D23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0</v>
+      </c>
+      <c r="G23" s="13">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13">
+        <v>1</v>
+      </c>
       <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
+      <c r="J23" s="13">
+        <v>0</v>
+      </c>
+      <c r="K23" s="13">
+        <v>1</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" s="15">
+        <v>1</v>
+      </c>
+      <c r="O23" s="15">
+        <v>1</v>
+      </c>
+      <c r="P23" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="15">
+        <v>1</v>
+      </c>
       <c r="R23" s="16"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
+      <c r="S23" s="17">
+        <v>-1</v>
+      </c>
+      <c r="T23" s="17">
+        <v>-1</v>
+      </c>
       <c r="U23" s="13"/>
-      <c r="V23" s="18"/>
-      <c r="W23" s="18"/>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="19"/>
+      <c r="V23" s="18">
+        <v>-1</v>
+      </c>
+      <c r="W23" s="18">
+        <v>-1</v>
+      </c>
+      <c r="X23" s="18">
+        <v>-1</v>
+      </c>
+      <c r="Y23" s="19">
+        <v>-1</v>
+      </c>
       <c r="Z23" s="20"/>
-      <c r="AA23" s="21"/>
-      <c r="AB23" s="21"/>
-      <c r="AC23" s="21"/>
-      <c r="AD23" s="21"/>
+      <c r="AA23" s="21">
+        <v>-1</v>
+      </c>
+      <c r="AB23" s="21">
+        <v>-2</v>
+      </c>
+      <c r="AC23" s="21">
+        <v>-3</v>
+      </c>
+      <c r="AD23" s="21">
+        <v>-4</v>
+      </c>
       <c r="AE23" s="21"/>
-      <c r="AF23" s="20"/>
+      <c r="AF23" s="20">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="22">
+        <v>-4</v>
+      </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18"/>
-      <c r="Y24" s="19"/>
-      <c r="Z24" s="20"/>
-      <c r="AA24" s="21"/>
-      <c r="AB24" s="21"/>
-      <c r="AC24" s="21"/>
-      <c r="AD24" s="21"/>
-      <c r="AE24" s="21"/>
-      <c r="AF24" s="20"/>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="18"/>
-      <c r="W25" s="18"/>
-      <c r="X25" s="18"/>
-      <c r="Y25" s="19"/>
-      <c r="Z25" s="20"/>
-      <c r="AA25" s="21"/>
-      <c r="AB25" s="21"/>
-      <c r="AC25" s="21"/>
-      <c r="AD25" s="21"/>
-      <c r="AE25" s="21"/>
-      <c r="AF25" s="20"/>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="18"/>
-      <c r="W26" s="18"/>
-      <c r="X26" s="18"/>
-      <c r="Y26" s="19"/>
-      <c r="Z26" s="20"/>
-      <c r="AA26" s="21"/>
-      <c r="AB26" s="21"/>
-      <c r="AC26" s="21"/>
-      <c r="AD26" s="21"/>
-      <c r="AE26" s="21"/>
-      <c r="AF26" s="20"/>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="18"/>
-      <c r="W27" s="18"/>
-      <c r="X27" s="18"/>
-      <c r="Y27" s="19"/>
-      <c r="Z27" s="20"/>
-      <c r="AA27" s="21"/>
-      <c r="AB27" s="21"/>
-      <c r="AC27" s="21"/>
-      <c r="AD27" s="21"/>
-      <c r="AE27" s="21"/>
-      <c r="AF27" s="20"/>
-    </row>
-    <row r="1048576" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B1048576" s="13">
+    <row r="1048572" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1048572" s="13">
         <v>0</v>
       </c>
     </row>

</xml_diff>